<commit_message>
ocr -> text ->df
</commit_message>
<xml_diff>
--- a/python/web_scrap_concepts/Ocr_Pdf/ocr_output.xlsx
+++ b/python/web_scrap_concepts/Ocr_Pdf/ocr_output.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,202 +434,249 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="B1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>#1</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr"/>
-      <c r="C1" t="inlineStr"/>
-      <c r="D1" t="inlineStr"/>
-      <c r="E1" t="inlineStr"/>
-      <c r="F1" t="inlineStr"/>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>student</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>=</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>{}</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>student["id"]</t>
-        </is>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>student</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>=</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>student["name"]</t>
-        </is>
+      <c r="A4" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>student["id"]</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>=</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>“taif™</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>student[“contact"]</t>
-        </is>
+      <c r="A5" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>student["name"]</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>=</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>1234567890</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>“taif™</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>student[“contact"]</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1234567890</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>for</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>keys,</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>values</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>in</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>student.</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>items():</t>
         </is>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>if</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>keys</t>
         </is>
       </c>
-      <c r="C7">
+      <c r="D8">
         <f>=</f>
         <v/>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>"name":</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>if</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>values</t>
         </is>
       </c>
-      <c r="C8">
+      <c r="D9">
         <f>=</f>
         <v/>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>“taif</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>print(“key</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>is</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>matched</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>with</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>value")</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>